<commit_message>
Implement password generation and hashing functions
</commit_message>
<xml_diff>
--- a/rsc/Classeur1.xlsx
+++ b/rsc/Classeur1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mathis\Documents\programmation\arc-en-ciel\rsc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB4EF45-D900-4CDE-8030-ED47FC8F7F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE048DA-3885-4573-B484-325B72FB4D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A58161D1-ACA7-4E84-B049-A4E5C06DA77A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="57">
   <si>
     <t>a</t>
   </si>
@@ -197,23 +197,23 @@
     <t>6 bits</t>
   </si>
   <si>
-    <t>42 bits</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>si 62 ou 63 alors on regarde a droite</t>
   </si>
   <si>
-    <t>si 62 ou 63 alors on fait un random entre 0 et 61</t>
+    <t>36 bits</t>
+  </si>
+  <si>
+    <t>si 62 ou 63 alors random entre 0 et 61</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,13 +221,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -242,16 +255,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -570,7 +588,7 @@
   <dimension ref="V1:AS64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F37" workbookViewId="0">
-      <selection activeCell="AP44" sqref="AP44"/>
+      <selection activeCell="AI51" sqref="AI51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,7 +647,7 @@
         <v>1</v>
       </c>
       <c r="AB2">
-        <f t="shared" ref="AB2:AC64" si="0">AA2+Z2*2+Y2*4+X2*8+W2*16+V2*32</f>
+        <f t="shared" ref="AB2:AB64" si="0">AA2+Z2*2+Y2*4+X2*8+W2*16+V2*32</f>
         <v>1</v>
       </c>
       <c r="AC2" s="1">
@@ -1742,24 +1760,24 @@
       <c r="AC43" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AE43" s="2">
+      <c r="AE43" s="3">
         <v>256</v>
       </c>
-      <c r="AF43" s="2"/>
-      <c r="AG43" s="2"/>
-      <c r="AH43" s="2"/>
-      <c r="AI43" s="2"/>
-      <c r="AJ43" s="2"/>
-      <c r="AK43" s="2"/>
-      <c r="AM43" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AN43" s="2"/>
-      <c r="AO43" s="2"/>
-      <c r="AP43" s="2"/>
-      <c r="AQ43" s="2"/>
-      <c r="AR43" s="2"/>
-      <c r="AS43" s="2"/>
+      <c r="AF43" s="3"/>
+      <c r="AG43" s="3"/>
+      <c r="AH43" s="3"/>
+      <c r="AI43" s="3"/>
+      <c r="AJ43" s="3"/>
+      <c r="AK43" s="3"/>
+      <c r="AM43" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN43" s="6"/>
+      <c r="AO43" s="6"/>
+      <c r="AP43" s="6"/>
+      <c r="AQ43" s="6"/>
+      <c r="AR43" s="6"/>
+      <c r="AS43" s="4"/>
     </row>
     <row r="44" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V44">
@@ -1788,28 +1806,28 @@
         <v>32</v>
       </c>
       <c r="AE44" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF44" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG44" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH44" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI44" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ44" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK44" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL44" t="s">
         <v>53</v>
-      </c>
-      <c r="AF44" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG44" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH44" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI44" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ44" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK44" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL44" t="s">
-        <v>54</v>
       </c>
       <c r="AM44" t="s">
         <v>52</v>
@@ -1829,9 +1847,6 @@
       <c r="AR44" t="s">
         <v>52</v>
       </c>
-      <c r="AS44" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="45" spans="22:45" ht="75" x14ac:dyDescent="0.25">
       <c r="V45">
@@ -1859,27 +1874,26 @@
       <c r="AC45" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AM45" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AN45" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO45" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AP45" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AQ45" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AR45" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS45" s="3" t="s">
+      <c r="AE45" s="5"/>
+      <c r="AM45" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN45" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO45" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP45" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ45" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR45" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="AS45" s="2"/>
     </row>
     <row r="46" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V46">
@@ -2391,7 +2405,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="AE43:AK43"/>
-    <mergeCell ref="AM43:AS43"/>
+    <mergeCell ref="AM43:AR43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>